<commit_message>
Liens Exemples CDA KO (#164) 0c0c399b46c20e0192a36bb5011f4c3a278d8a76
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
+++ b/ig/main/StructureDefinition-esms-bundle-resultat-recherche-decision-evaluation.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1798" uniqueCount="282">
   <si>
     <t>Property</t>
   </si>
@@ -650,10 +650,6 @@
   </si>
   <si>
     <t>Usually, this is used for documents other than those defined by FHIR.</t>
-  </si>
-  <si>
-    <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.`div`.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}regle-Contenu:Le transport des données devient obligatoire lorsque la ressource complète est transportée, le champs data doit alors être rempli {content.attachment.data.exists()}regle-NomPieceJointe:Le nom de la pièce jointe doit être  : "Document Individu et décision" ou "Document évaluation" {content.attachment.title='Document Individu et décision' or content.attachment.title='Document évaluation'}</t>
   </si>
   <si>
     <t>Document[classCode="DOC" and moodCode="EVN"]</t>
@@ -3864,16 +3860,16 @@
         <v>76</v>
       </c>
       <c r="AJ23" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AK23" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL23" t="s" s="2">
         <v>201</v>
       </c>
-      <c r="AK23" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL23" t="s" s="2">
+      <c r="AM23" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="AM23" t="s" s="2">
-        <v>203</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>76</v>
@@ -3881,10 +3877,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -3910,10 +3906,10 @@
         <v>148</v>
       </c>
       <c r="L24" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="M24" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>206</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
@@ -3964,7 +3960,7 @@
         <v>76</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>77</v>
@@ -3973,7 +3969,7 @@
         <v>86</v>
       </c>
       <c r="AI24" t="s" s="2">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AJ24" t="s" s="2">
         <v>99</v>
@@ -3993,10 +3989,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4105,10 +4101,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -4219,10 +4215,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4335,10 +4331,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -4364,13 +4360,13 @@
         <v>108</v>
       </c>
       <c r="L28" t="s" s="2">
+        <v>211</v>
+      </c>
+      <c r="M28" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="M28" t="s" s="2">
+      <c r="N28" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>214</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -4399,11 +4395,11 @@
         <v>130</v>
       </c>
       <c r="Y28" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="Z28" t="s" s="2">
         <v>215</v>
       </c>
-      <c r="Z28" t="s" s="2">
-        <v>216</v>
-      </c>
       <c r="AA28" t="s" s="2">
         <v>76</v>
       </c>
@@ -4420,7 +4416,7 @@
         <v>76</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>77</v>
@@ -4449,10 +4445,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -4475,16 +4471,16 @@
         <v>87</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>218</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="M29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>220</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>221</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
@@ -4534,7 +4530,7 @@
         <v>76</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>77</v>
@@ -4563,10 +4559,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -4592,10 +4588,10 @@
         <v>148</v>
       </c>
       <c r="L30" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>223</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>224</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -4646,7 +4642,7 @@
         <v>76</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>77</v>
@@ -4655,7 +4651,7 @@
         <v>86</v>
       </c>
       <c r="AI30" t="s" s="2">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="AJ30" t="s" s="2">
         <v>99</v>
@@ -4675,10 +4671,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -4787,10 +4783,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -4901,10 +4897,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5017,10 +5013,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5046,10 +5042,10 @@
         <v>108</v>
       </c>
       <c r="L34" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>231</v>
       </c>
       <c r="N34" t="s" s="2">
         <v>177</v>
@@ -5081,11 +5077,11 @@
         <v>130</v>
       </c>
       <c r="Y34" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="Z34" t="s" s="2">
         <v>232</v>
       </c>
-      <c r="Z34" t="s" s="2">
-        <v>233</v>
-      </c>
       <c r="AA34" t="s" s="2">
         <v>76</v>
       </c>
@@ -5102,7 +5098,7 @@
         <v>76</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>86</v>
@@ -5131,10 +5127,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5160,13 +5156,13 @@
         <v>101</v>
       </c>
       <c r="L35" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="M35" t="s" s="2">
         <v>235</v>
       </c>
-      <c r="M35" t="s" s="2">
+      <c r="N35" t="s" s="2">
         <v>236</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>237</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
@@ -5216,7 +5212,7 @@
         <v>76</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>86</v>
@@ -5245,10 +5241,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5274,10 +5270,10 @@
         <v>153</v>
       </c>
       <c r="L36" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="M36" t="s" s="2">
         <v>239</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="N36" t="s" s="2">
         <v>177</v>
@@ -5330,7 +5326,7 @@
         <v>76</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>77</v>
@@ -5359,10 +5355,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5388,13 +5384,13 @@
         <v>135</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M37" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="N37" t="s" s="2">
         <v>242</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>243</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
@@ -5444,7 +5440,7 @@
         <v>76</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>77</v>
@@ -5473,10 +5469,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -5502,10 +5498,10 @@
         <v>153</v>
       </c>
       <c r="L38" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="M38" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>246</v>
       </c>
       <c r="N38" t="s" s="2">
         <v>177</v>
@@ -5558,7 +5554,7 @@
         <v>76</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>77</v>
@@ -5587,10 +5583,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -5616,10 +5612,10 @@
         <v>153</v>
       </c>
       <c r="L39" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="M39" t="s" s="2">
         <v>248</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>249</v>
       </c>
       <c r="N39" t="s" s="2">
         <v>177</v>
@@ -5672,7 +5668,7 @@
         <v>76</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>77</v>
@@ -5701,10 +5697,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -5730,10 +5726,10 @@
         <v>148</v>
       </c>
       <c r="L40" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="M40" t="s" s="2">
         <v>251</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>252</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -5784,7 +5780,7 @@
         <v>76</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>77</v>
@@ -5793,7 +5789,7 @@
         <v>86</v>
       </c>
       <c r="AI40" t="s" s="2">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AJ40" t="s" s="2">
         <v>99</v>
@@ -5813,10 +5809,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -5925,10 +5921,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6039,10 +6035,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6155,10 +6151,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6184,10 +6180,10 @@
         <v>153</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="M44" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>259</v>
       </c>
       <c r="N44" t="s" s="2">
         <v>177</v>
@@ -6240,7 +6236,7 @@
         <v>76</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>86</v>
@@ -6269,10 +6265,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6298,10 +6294,10 @@
         <v>101</v>
       </c>
       <c r="L45" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="M45" t="s" s="2">
         <v>261</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>262</v>
       </c>
       <c r="N45" t="s" s="2">
         <v>181</v>
@@ -6354,7 +6350,7 @@
         <v>76</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>77</v>
@@ -6383,10 +6379,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -6412,13 +6408,13 @@
         <v>153</v>
       </c>
       <c r="L46" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="M46" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="M46" t="s" s="2">
+      <c r="N46" t="s" s="2">
         <v>265</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>266</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -6468,7 +6464,7 @@
         <v>76</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>77</v>
@@ -6497,10 +6493,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -6526,13 +6522,13 @@
         <v>135</v>
       </c>
       <c r="L47" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>268</v>
       </c>
-      <c r="M47" t="s" s="2">
+      <c r="N47" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>270</v>
       </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
@@ -6582,7 +6578,7 @@
         <v>76</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>77</v>
@@ -6611,10 +6607,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -6637,16 +6633,16 @@
         <v>87</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>272</v>
       </c>
-      <c r="L48" t="s" s="2">
+      <c r="M48" t="s" s="2">
         <v>273</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>274</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>275</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -6696,7 +6692,7 @@
         <v>76</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>77</v>
@@ -6714,7 +6710,7 @@
         <v>76</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>76</v>
@@ -6725,10 +6721,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -6751,19 +6747,19 @@
         <v>87</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>278</v>
       </c>
-      <c r="L49" t="s" s="2">
+      <c r="M49" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="M49" t="s" s="2">
+      <c r="N49" t="s" s="2">
         <v>280</v>
       </c>
-      <c r="N49" t="s" s="2">
+      <c r="O49" t="s" s="2">
         <v>281</v>
-      </c>
-      <c r="O49" t="s" s="2">
-        <v>282</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>76</v>
@@ -6812,7 +6808,7 @@
         <v>76</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>77</v>

</xml_diff>